<commit_message>
some changes in style
</commit_message>
<xml_diff>
--- a/MDR_tabela.xlsx
+++ b/MDR_tabela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Pacote</t>
   </si>
@@ -73,9 +73,6 @@
     <t>UDTB - Updated Databook</t>
   </si>
   <si>
-    <t>Teste</t>
-  </si>
-  <si>
     <t>Umbilical</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>ANM</t>
   </si>
   <si>
-    <t>Luis</t>
-  </si>
-  <si>
     <t>UMB - Umbilical</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t>PLM - Manifold &amp; PLEM</t>
-  </si>
-  <si>
-    <t>XTE - XT &amp; Tools</t>
   </si>
 </sst>
 </file>
@@ -455,13 +446,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,146 +510,137 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -703,26 +685,6 @@
         <v>0</v>
       </c>
       <c r="S4" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>